<commit_message>
refactor(xlsx-loader): :recycle: change variables structure, add 'event'
BREAKING CHANGE: modify variables data structure
</commit_message>
<xml_diff>
--- a/packages/xlsx-loader/__tests__/variables.xlsx
+++ b/packages/xlsx-loader/__tests__/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/GitHub/epicagency/@snitchy/packages/xlsx-loader/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/GitHub/epicagency/@snitchy/packages/xlsx-loader/__tests__/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A96E21-9B5A-0D43-B329-150B3243FEBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A39B4D-41D3-104A-96FA-D67902EDA3D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{D3F33F63-55B0-9B40-98A2-7C728CAADFC9}"/>
+    <workbookView xWindow="34280" yWindow="600" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{D3F33F63-55B0-9B40-98A2-7C728CAADFC9}"/>
   </bookViews>
   <sheets>
     <sheet name="pages" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>title</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>somthingCustom</t>
+  </si>
+  <si>
+    <t>page-load</t>
+  </si>
+  <si>
+    <t>page-other</t>
   </si>
 </sst>
 </file>
@@ -535,21 +541,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860E35F6-087B-0B43-B463-367669A09B1D}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="23.83203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="6" width="23.83203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -557,22 +563,25 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -580,48 +589,56 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -629,26 +646,32 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -656,10 +679,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -671,20 +697,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042B383B-9945-264D-8764-8A92F8BE5F38}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="29" style="3" customWidth="1"/>
-    <col min="6" max="7" width="23.83203125" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="6" width="29" style="3" customWidth="1"/>
+    <col min="7" max="8" width="23.83203125" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -692,22 +718,25 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -715,93 +744,78 @@
         <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+    <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    <row r="7" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+      <c r="F7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: :recycle: End of refactoring
Rewrite and optimize code, more tests, update config for easier testing

BREAKING CHANGE: update dependencies and finalize variables data structure
</commit_message>
<xml_diff>
--- a/packages/xlsx-loader/__tests__/variables.xlsx
+++ b/packages/xlsx-loader/__tests__/variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/GitHub/epicagency/@snitchy/packages/xlsx-loader/__tests__/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A39B4D-41D3-104A-96FA-D67902EDA3D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B08CF4-9355-FE49-8035-8486EADCD65E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34280" yWindow="600" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{D3F33F63-55B0-9B40-98A2-7C728CAADFC9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{D3F33F63-55B0-9B40-98A2-7C728CAADFC9}"/>
   </bookViews>
   <sheets>
     <sheet name="pages" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>title</t>
   </si>
@@ -107,9 +107,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>actions</t>
   </si>
   <si>
@@ -146,13 +143,19 @@
     <t>decription</t>
   </si>
   <si>
-    <t>somthingCustom</t>
-  </si>
-  <si>
     <t>page-load</t>
   </si>
   <si>
-    <t>page-other</t>
+    <t>page-refresh</t>
+  </si>
+  <si>
+    <t>offline</t>
+  </si>
+  <si>
+    <t>somethingDifferent</t>
+  </si>
+  <si>
+    <t>somethingCustom</t>
   </si>
 </sst>
 </file>
@@ -541,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860E35F6-087B-0B43-B463-367669A09B1D}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -569,16 +572,16 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -589,7 +592,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
@@ -614,78 +617,91 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="5" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="B8" s="3" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -699,13 +715,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042B383B-9945-264D-8764-8A92F8BE5F38}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="29" style="3" customWidth="1"/>
+    <col min="1" max="6" width="23" style="3" customWidth="1"/>
     <col min="7" max="8" width="23.83203125" style="4" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="4"/>
   </cols>
@@ -724,16 +740,16 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -741,7 +757,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>15</v>
@@ -758,18 +774,18 @@
         <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -794,7 +810,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -816,7 +832,7 @@
         <v>20</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -835,7 +851,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>